<commit_message>
Added temporary data files for adding and installing lists
</commit_message>
<xml_diff>
--- a/GameGetter/Data/Input/SteamGameList.xlsx
+++ b/GameGetter/Data/Input/SteamGameList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\201019-UTA0UiPath\Team3-P2\SteamAddProject\Data\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\201019-UTA0UiPath\Team3-P2\GameGetter\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB17CAF2-9B6A-4A51-A5FF-C283FBC61729}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51B9D9B-0F03-4DC3-821D-9B3A50A46373}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5160" yWindow="4050" windowWidth="28800" windowHeight="15435" xr2:uid="{4CF00BEE-FD2A-4CB3-AFE8-B7D834D8E461}"/>
+    <workbookView xWindow="5190" yWindow="3300" windowWidth="28800" windowHeight="15435" xr2:uid="{4CF00BEE-FD2A-4CB3-AFE8-B7D834D8E461}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,23 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="34">
-  <si>
-    <t>Game Title</t>
-  </si>
-  <si>
-    <t>Add</t>
-  </si>
-  <si>
-    <t>Install</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Toast Defense</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Tiny Toy Tanks</t>
   </si>
   <si>
@@ -131,10 +119,10 @@
     <t>Cubiscape 2</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>Apex Legends</t>
+  </si>
+  <si>
+    <t>Title</t>
   </si>
 </sst>
 </file>
@@ -486,353 +474,167 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CDCD57F-7456-4936-A6B7-AF944866C104}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:A31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>16</v>
       </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="B15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>19</v>
       </c>
-      <c r="B18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>20</v>
       </c>
-      <c r="B19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>21</v>
       </c>
-      <c r="B20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>22</v>
       </c>
-      <c r="B21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>23</v>
       </c>
-      <c r="B22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>24</v>
       </c>
-      <c r="B24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>25</v>
       </c>
-      <c r="B25" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>26</v>
       </c>
-      <c r="B26" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>27</v>
-      </c>
-      <c r="B27" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
renamed table filter workflow to reflect purpose
</commit_message>
<xml_diff>
--- a/GameGetter/Data/Input/SteamGameList.xlsx
+++ b/GameGetter/Data/Input/SteamGameList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\Team3-P2\GameGetter\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8A30A7-9B8A-447F-93C5-2518D67BEA7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DB85C5-33C2-420E-85BF-44C524568AC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4CF00BEE-FD2A-4CB3-AFE8-B7D834D8E461}"/>
+    <workbookView xWindow="4920" yWindow="2892" windowWidth="17280" windowHeight="8964" xr2:uid="{4CF00BEE-FD2A-4CB3-AFE8-B7D834D8E461}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Toast Defense</t>
   </si>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>Title</t>
-  </si>
-  <si>
-    <t>Meant To Fail</t>
   </si>
 </sst>
 </file>
@@ -477,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CDCD57F-7456-4936-A6B7-AF944866C104}">
-  <dimension ref="A1:A32"/>
+  <dimension ref="A1:A31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -640,11 +637,6 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>30</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>